<commit_message>
Inicio planes de prueba de hardware, ordene algunas carpetas para que tablas y graficos esten cerca
</commit_message>
<xml_diff>
--- a/Documentación/Tablas/9-2 Especificación de Tests.xlsx
+++ b/Documentación/Tablas/9-2 Especificación de Tests.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27143A60-821B-4058-A2F7-0524E4E79827}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{623ADBA4-A8DB-460C-96D2-72C4A9BCF639}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="8.2 Especificación de tests" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="104">
   <si>
     <t>Descripción</t>
   </si>
@@ -158,12 +158,6 @@
     <t>T-INT-DIM-02</t>
   </si>
   <si>
-    <t>T-INT-COM-02</t>
-  </si>
-  <si>
-    <t>T-INT-FUNC-09</t>
-  </si>
-  <si>
     <t>T-INT-MEC-01</t>
   </si>
   <si>
@@ -171,11 +165,6 @@
   </si>
   <si>
     <t>T-INT-MEC-03</t>
-  </si>
-  <si>
-    <t>T-INT-COM-01
-T-INT-DIM-01
-T-INT-DIM-02</t>
   </si>
   <si>
     <t>T-INT-DATA-02</t>
@@ -453,6 +442,25 @@
 \tabitem Conectar la base a una computadora y abrir el puerto serie correspondiente a la base.
 \tabitem Interactuar con la interfaz de obtención de datos propia del dispositivo.
 \tabitem Confirmar la recepción de datos.</t>
+  </si>
+  <si>
+    <t>T-INT-FUNC-01
+T-INT-FUNC-02
+T-INT-FUNC-03</t>
+  </si>
+  <si>
+    <t>T-INT-FUNC-04
+T-INT-FUNC-05
+T-INT-FUNC-06</t>
+  </si>
+  <si>
+    <t>T-INT-DIM-01
+T-INT-DIM-02</t>
+  </si>
+  <si>
+    <t>T-INT-MEC-01
+T-INT-MEC-02
+T-INT-MEC-03</t>
   </si>
 </sst>
 </file>
@@ -568,7 +576,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -582,21 +590,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -616,20 +636,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -919,7 +926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7EAD9908-3DB8-46A4-94BE-5CD81246CF66}">
   <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="D17" sqref="A1:D19"/>
     </sheetView>
   </sheetViews>
@@ -955,7 +962,7 @@
       <c r="C2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D2" s="17" t="s">
         <v>1</v>
       </c>
     </row>
@@ -969,7 +976,7 @@
       <c r="C3" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="14"/>
+      <c r="D3" s="18"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
@@ -978,10 +985,10 @@
       <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="10" t="s">
+      <c r="C4" s="14" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="14"/>
+      <c r="D4" s="18"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
@@ -990,8 +997,8 @@
       <c r="B5" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="11"/>
-      <c r="D5" s="14"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="18"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
@@ -1000,8 +1007,8 @@
       <c r="B6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C6" s="12"/>
-      <c r="D6" s="14"/>
+      <c r="C6" s="16"/>
+      <c r="D6" s="18"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
@@ -1010,10 +1017,10 @@
       <c r="B7" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D7" s="14"/>
+      <c r="C7" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="D7" s="18"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
@@ -1022,10 +1029,8 @@
       <c r="B8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D8" s="14"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="18"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
@@ -1034,22 +1039,20 @@
       <c r="B9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" s="15"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C9" s="16"/>
+      <c r="D9" s="19"/>
+    </row>
+    <row r="10" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="13" t="s">
+      <c r="C10" s="4" t="s">
+        <v>101</v>
+      </c>
+      <c r="D10" s="17" t="s">
         <v>2</v>
       </c>
     </row>
@@ -1063,7 +1066,7 @@
       <c r="C11" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D11" s="15"/>
+      <c r="D11" s="19"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
@@ -1075,7 +1078,7 @@
       <c r="C12" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="13" t="s">
         <v>3</v>
       </c>
     </row>
@@ -1087,84 +1090,84 @@
         <v>20</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D13" s="5"/>
+        <v>37</v>
+      </c>
+      <c r="D13" s="13"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="5" t="s">
+      <c r="C14" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="13" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
+      <c r="C15" s="13"/>
+      <c r="D15" s="13"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C16" s="5"/>
-      <c r="D16" s="5"/>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C16" s="13"/>
+      <c r="D16" s="13"/>
+    </row>
+    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="C17" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="5" t="s">
+      <c r="C17" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="D17" s="13" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D18" s="5"/>
+        <v>44</v>
+      </c>
+      <c r="D18" s="13"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D19" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D19" s="13"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="8">
     <mergeCell ref="D17:D19"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D2:D9"/>
@@ -1172,6 +1175,7 @@
     <mergeCell ref="C14:C16"/>
     <mergeCell ref="D12:D13"/>
     <mergeCell ref="D14:D16"/>
+    <mergeCell ref="C7:C9"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1194,36 +1198,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>48</v>
+      <c r="A1" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>82</v>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>49</v>
+        <v>63</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>50</v>
+        <v>80</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -1247,91 +1251,91 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>48</v>
+      <c r="A1" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>82</v>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>67</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>52</v>
+        <v>83</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>68</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>53</v>
+        <v>84</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>69</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>54</v>
+        <v>85</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>55</v>
+        <v>86</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="B6" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>56</v>
+        <v>87</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>53</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="B7" s="9" t="s">
-        <v>72</v>
-      </c>
-      <c r="C7" s="16" t="s">
-        <v>57</v>
+        <v>88</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C7" s="9" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="B8" s="9" t="s">
-        <v>73</v>
-      </c>
-      <c r="C8" s="16" t="s">
-        <v>58</v>
+        <v>89</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
@@ -1341,7 +1345,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0611DCA8-B494-4BF5-A555-ED9E5089E1A0}">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
@@ -1355,66 +1359,56 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>48</v>
+      <c r="A1" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>82</v>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="150" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>59</v>
+        <v>99</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="18"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="20"/>
+      <c r="A3" s="10"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="12"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="18"/>
-      <c r="B4" s="19"/>
-      <c r="C4" s="21"/>
+      <c r="A4" s="10"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="7"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="18"/>
-      <c r="B5" s="19"/>
-      <c r="C5" s="21"/>
+      <c r="A5" s="10"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="7"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="18"/>
-      <c r="B6" s="19"/>
-      <c r="C6" s="21"/>
+      <c r="A6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="7"/>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="18"/>
-      <c r="B7" s="19"/>
-      <c r="C7" s="21"/>
+      <c r="A7" s="10"/>
+      <c r="B7" s="11"/>
+      <c r="C7" s="7"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="18"/>
-      <c r="B8" s="19"/>
-      <c r="C8" s="21"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="17"/>
-      <c r="B9" s="17"/>
-      <c r="C9" s="17"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="17"/>
-      <c r="B10" s="17"/>
-      <c r="C10" s="17"/>
+      <c r="A8" s="10"/>
+      <c r="B8" s="11"/>
+      <c r="C8" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1437,73 +1431,73 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>48</v>
+      <c r="A1" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>82</v>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>74</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>60</v>
+        <v>91</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>61</v>
+        <v>72</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>62</v>
+        <v>73</v>
+      </c>
+      <c r="C4" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>62</v>
+        <v>74</v>
+      </c>
+      <c r="C5" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="210" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="C6" s="16" t="s">
-        <v>62</v>
+        <v>75</v>
+      </c>
+      <c r="C6" s="9" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C7" s="8"/>
+      <c r="C7" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1514,7 +1508,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2780F216-54B4-4021-B76B-7E398446177D}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection sqref="A1:C4"/>
     </sheetView>
   </sheetViews>
@@ -1526,51 +1520,51 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="6" t="s">
-        <v>48</v>
+      <c r="A1" s="5" t="s">
+        <v>45</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="6" t="s">
-        <v>82</v>
+      <c r="C1" s="5" t="s">
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="B2" s="9" t="s">
-        <v>79</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>63</v>
+        <v>96</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>64</v>
+        <v>77</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="C4" s="7" t="s">
-        <v>65</v>
+        <v>78</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C5" s="8"/>
+      <c r="C5" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>